<commit_message>
eieio: Update aggregate categories
</commit_message>
<xml_diff>
--- a/emissions/slca/eieio/data/aggregates_small_test.xlsx
+++ b/emissions/slca/eieio/data/aggregates_small_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bea" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="663">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -1526,67 +1526,61 @@
     <t xml:space="preserve">Elec. Util., Coal</t>
   </si>
   <si>
-    <t xml:space="preserve">Elec. Util., Other</t>
-  </si>
-  <si>
     <t xml:space="preserve">Petroleum Prod. Production</t>
   </si>
   <si>
     <t xml:space="preserve">Petroleum Prod.</t>
   </si>
   <si>
+    <t xml:space="preserve">Industrial Fuel Comb.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrial</t>
+  </si>
+  <si>
     <t xml:space="preserve">0010201901</t>
   </si>
   <si>
-    <t xml:space="preserve">Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industrial Fuel Comb.</t>
+    <t xml:space="preserve">Other Industrial Processes</t>
   </si>
   <si>
     <t xml:space="preserve">0030280001</t>
   </si>
   <si>
-    <t xml:space="preserve">Other Industrial Processes</t>
+    <t xml:space="preserve">Metals Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal Proc.</t>
   </si>
   <si>
     <t xml:space="preserve">0030200408</t>
   </si>
   <si>
-    <t xml:space="preserve">Metals Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metal Proc.</t>
+    <t xml:space="preserve">Mining &amp; Mineral Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mining</t>
   </si>
   <si>
     <t xml:space="preserve">0010200603</t>
   </si>
   <si>
-    <t xml:space="preserve">Mining &amp; Mineral Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mining</t>
-  </si>
-  <si>
     <t xml:space="preserve">Industrial Solvents</t>
   </si>
   <si>
-    <t xml:space="preserve">Consumer Solvents</t>
+    <t xml:space="preserve">Highway Veh., Heavy Duty, Diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy Hwy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highway Veh., Light Duty, Gas</t>
   </si>
   <si>
     <t xml:space="preserve">0020200252</t>
   </si>
   <si>
-    <t xml:space="preserve">Highway Veh., Heavy Duty, Diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heavy Hwy</t>
-  </si>
-  <si>
     <t xml:space="preserve">0010100203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highway Veh., Light Duty, Gas</t>
   </si>
   <si>
     <t xml:space="preserve">0010100901</t>
@@ -2133,7 +2127,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2160,10 +2154,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2215,8 +2205,8 @@
   </sheetPr>
   <dimension ref="A1:J390"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2600,7 +2590,7 @@
       <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="7" t="str">
+      <c r="C15" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -2732,7 +2722,7 @@
       <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="7" t="str">
+      <c r="C21" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -2798,7 +2788,7 @@
       <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="7" t="str">
+      <c r="C24" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -3110,10 +3100,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E38" s="8" t="n">
+      <c r="E38" s="7" t="n">
         <v>321100</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="8" t="s">
         <v>65</v>
       </c>
       <c r="G38" s="0" t="str">
@@ -3132,10 +3122,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E39" s="8" t="n">
+      <c r="E39" s="7" t="n">
         <v>321200</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="8" t="s">
         <v>66</v>
       </c>
       <c r="G39" s="0" t="str">
@@ -3154,10 +3144,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E40" s="8" t="n">
+      <c r="E40" s="7" t="n">
         <v>321910</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G40" s="0" t="str">
@@ -3176,10 +3166,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="8" t="s">
         <v>69</v>
       </c>
       <c r="G41" s="0" t="str">
@@ -3198,10 +3188,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E42" s="8" t="n">
+      <c r="E42" s="7" t="n">
         <v>327100</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F42" s="8" t="s">
         <v>70</v>
       </c>
       <c r="G42" s="0" t="str">
@@ -3220,10 +3210,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E43" s="8" t="n">
+      <c r="E43" s="7" t="n">
         <v>327200</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G43" s="0" t="str">
@@ -3242,10 +3232,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E44" s="8" t="n">
+      <c r="E44" s="7" t="n">
         <v>327310</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G44" s="0" t="str">
@@ -3795,7 +3785,7 @@
       <c r="E69" s="6" t="n">
         <v>332320</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F69" s="9" t="s">
         <v>102</v>
       </c>
       <c r="G69" s="0" t="str">
@@ -3814,10 +3804,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E70" s="11" t="n">
+      <c r="E70" s="10" t="n">
         <v>332410</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="11" t="s">
         <v>103</v>
       </c>
       <c r="G70" s="0" t="str">
@@ -3858,10 +3848,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E72" s="11" t="n">
+      <c r="E72" s="10" t="n">
         <v>332430</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="F72" s="10" t="s">
         <v>105</v>
       </c>
       <c r="G72" s="0" t="str">
@@ -3902,10 +3892,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E74" s="11" t="n">
+      <c r="E74" s="10" t="n">
         <v>332600</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="11" t="s">
         <v>107</v>
       </c>
       <c r="G74" s="0" t="str">
@@ -3924,10 +3914,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E75" s="11" t="n">
+      <c r="E75" s="10" t="n">
         <v>332710</v>
       </c>
-      <c r="F75" s="11" t="s">
+      <c r="F75" s="10" t="s">
         <v>108</v>
       </c>
       <c r="G75" s="0" t="str">
@@ -3946,10 +3936,10 @@
         <f aca="false">$J$7</f>
         <v>Goods</v>
       </c>
-      <c r="E76" s="11" t="n">
+      <c r="E76" s="10" t="n">
         <v>332720</v>
       </c>
-      <c r="F76" s="11" t="s">
+      <c r="F76" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G76" s="0" t="str">
@@ -4125,7 +4115,7 @@
       <c r="E84" s="6" t="n">
         <v>333111</v>
       </c>
-      <c r="F84" s="9" t="s">
+      <c r="F84" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G84" s="0" t="str">
@@ -4147,7 +4137,7 @@
       <c r="E85" s="6" t="n">
         <v>333112</v>
       </c>
-      <c r="F85" s="9" t="s">
+      <c r="F85" s="8" t="s">
         <v>121</v>
       </c>
       <c r="G85" s="0" t="str">
@@ -4169,7 +4159,7 @@
       <c r="E86" s="6" t="n">
         <v>333120</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F86" s="8" t="s">
         <v>122</v>
       </c>
       <c r="G86" s="0" t="str">
@@ -4191,7 +4181,7 @@
       <c r="E87" s="6" t="n">
         <v>333130</v>
       </c>
-      <c r="F87" s="9" t="s">
+      <c r="F87" s="8" t="s">
         <v>123</v>
       </c>
       <c r="G87" s="0" t="str">
@@ -4213,7 +4203,7 @@
       <c r="E88" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F88" s="9" t="s">
+      <c r="F88" s="8" t="s">
         <v>125</v>
       </c>
       <c r="G88" s="0" t="str">
@@ -5636,7 +5626,7 @@
       <c r="B153" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C153" s="7" t="str">
+      <c r="C153" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5658,7 +5648,7 @@
       <c r="B154" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C154" s="7" t="str">
+      <c r="C154" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5680,7 +5670,7 @@
       <c r="B155" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C155" s="7" t="str">
+      <c r="C155" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5702,7 +5692,7 @@
       <c r="B156" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C156" s="7" t="str">
+      <c r="C156" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5724,7 +5714,7 @@
       <c r="B157" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C157" s="7" t="str">
+      <c r="C157" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5746,7 +5736,7 @@
       <c r="B158" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C158" s="7" t="str">
+      <c r="C158" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5768,7 +5758,7 @@
       <c r="B159" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C159" s="7" t="str">
+      <c r="C159" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5790,7 +5780,7 @@
       <c r="B160" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C160" s="7" t="str">
+      <c r="C160" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5812,7 +5802,7 @@
       <c r="B161" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C161" s="7" t="str">
+      <c r="C161" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5834,7 +5824,7 @@
       <c r="B162" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C162" s="7" t="str">
+      <c r="C162" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5856,7 +5846,7 @@
       <c r="B163" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C163" s="7" t="str">
+      <c r="C163" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5878,7 +5868,7 @@
       <c r="B164" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C164" s="7" t="str">
+      <c r="C164" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5900,7 +5890,7 @@
       <c r="B165" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C165" s="7" t="str">
+      <c r="C165" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5922,7 +5912,7 @@
       <c r="B166" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C166" s="7" t="str">
+      <c r="C166" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5944,7 +5934,7 @@
       <c r="B167" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C167" s="7" t="str">
+      <c r="C167" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -5966,7 +5956,7 @@
       <c r="B168" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C168" s="7" t="str">
+      <c r="C168" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -6032,7 +6022,7 @@
       <c r="B171" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C171" s="7" t="str">
+      <c r="C171" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -6054,7 +6044,7 @@
       <c r="B172" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C172" s="7" t="str">
+      <c r="C172" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -6076,7 +6066,7 @@
       <c r="B173" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C173" s="7" t="str">
+      <c r="C173" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -6098,7 +6088,7 @@
       <c r="B174" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C174" s="7" t="str">
+      <c r="C174" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -6120,7 +6110,7 @@
       <c r="B175" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C175" s="7" t="str">
+      <c r="C175" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -6142,7 +6132,7 @@
       <c r="B176" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C176" s="7" t="str">
+      <c r="C176" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -7616,7 +7606,7 @@
       <c r="B243" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C243" s="7" t="str">
+      <c r="C243" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -7638,7 +7628,7 @@
       <c r="B244" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="C244" s="7" t="str">
+      <c r="C244" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -8276,7 +8266,7 @@
       <c r="B273" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="C273" s="7" t="str">
+      <c r="C273" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -10410,7 +10400,7 @@
       <c r="B370" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="C370" s="7" t="str">
+      <c r="C370" s="2" t="str">
         <f aca="false">$J$6</f>
         <v>Trans.</v>
       </c>
@@ -10883,8 +10873,8 @@
   </sheetPr>
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H172" activeCellId="0" sqref="H172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10900,23 +10890,23 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>489</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>488</v>
       </c>
     </row>
@@ -11009,7 +10999,7 @@
         <v>501</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>502</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>2203420080</v>
@@ -11020,16 +11010,16 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="G9" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>504</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11037,7 +11027,7 @@
         <v>506</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>507</v>
@@ -11051,35 +11041,35 @@
         <v>508</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>2415000000</v>
@@ -11093,7 +11083,7 @@
         <v>515</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>492</v>
+        <v>516</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>2401065000</v>
@@ -11104,57 +11094,45 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="G16" s="0" t="s">
         <v>519</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>520</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>494</v>
-      </c>
       <c r="G17" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="14" t="s">
-        <v>523</v>
+      <c r="G18" s="13" t="s">
+        <v>521</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G19" s="0" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>494</v>
@@ -11162,15 +11140,15 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G20" s="0" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G21" s="0" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>494</v>
@@ -11178,7 +11156,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G22" s="0" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>494</v>
@@ -11186,7 +11164,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="0" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>494</v>
@@ -11194,7 +11172,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="0" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>494</v>
@@ -11202,7 +11180,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G25" s="0" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>494</v>
@@ -11210,7 +11188,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="0" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>494</v>
@@ -11218,15 +11196,15 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="0" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="14" t="s">
-        <v>533</v>
+      <c r="G28" s="13" t="s">
+        <v>531</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>494</v>
@@ -11234,7 +11212,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="0" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>494</v>
@@ -11242,7 +11220,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G30" s="0" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>494</v>
@@ -11250,7 +11228,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G31" s="0" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>494</v>
@@ -11258,7 +11236,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G32" s="0" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>494</v>
@@ -11266,7 +11244,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G33" s="0" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>494</v>
@@ -11274,7 +11252,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>494</v>
@@ -11282,7 +11260,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G35" s="0" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>494</v>
@@ -11290,7 +11268,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G36" s="0" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>494</v>
@@ -11298,7 +11276,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G37" s="0" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>494</v>
@@ -11306,7 +11284,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G38" s="0" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>494</v>
@@ -11314,23 +11292,23 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G39" s="0" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G40" s="0" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G41" s="0" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H41" s="0" t="s">
         <v>494</v>
@@ -11338,7 +11316,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G42" s="0" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H42" s="0" t="s">
         <v>494</v>
@@ -11346,167 +11324,167 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G43" s="0" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G44" s="0" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G45" s="0" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="0" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G47" s="0" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G48" s="0" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G49" s="0" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G50" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="13" t="s">
+        <v>554</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="13" t="s">
         <v>555</v>
       </c>
-      <c r="H50" s="0" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G51" s="14" t="s">
-        <v>556</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G52" s="14" t="s">
-        <v>557</v>
-      </c>
       <c r="H52" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G53" s="0" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G54" s="0" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G55" s="0" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G56" s="0" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G57" s="0" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G58" s="0" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G59" s="0" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G60" s="0" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G61" s="0" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G62" s="0" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G63" s="0" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H63" s="0" t="s">
         <v>494</v>
@@ -11514,175 +11492,175 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G64" s="0" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G65" s="0" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G66" s="0" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G67" s="0" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G68" s="0" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G69" s="0" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G70" s="0" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G71" s="0" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G72" s="0" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G73" s="0" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G74" s="0" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G75" s="0" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G76" s="0" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G77" s="0" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G78" s="0" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G79" s="0" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G80" s="0" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G81" s="0" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G82" s="0" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G83" s="0" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G84" s="0" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G85" s="0" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="H85" s="0" t="s">
         <v>494</v>
@@ -11690,47 +11668,47 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G86" s="0" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G87" s="0" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G88" s="0" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G89" s="0" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G90" s="0" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G91" s="0" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H91" s="0" t="s">
         <v>494</v>
@@ -11738,31 +11716,31 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G92" s="0" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G93" s="0" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G94" s="0" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G95" s="0" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H95" s="0" t="s">
         <v>494</v>
@@ -11770,79 +11748,79 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G96" s="0" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="H96" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G97" s="0" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H97" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G98" s="0" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H98" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G99" s="0" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H99" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G100" s="0" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="H100" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G101" s="0" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H101" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G102" s="0" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H102" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G103" s="0" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="H103" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G104" s="0" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H104" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G105" s="0" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="H105" s="0" t="s">
         <v>494</v>
@@ -11850,223 +11828,223 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G106" s="0" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H106" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G107" s="0" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H107" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G108" s="0" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="H108" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G109" s="0" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H109" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G110" s="0" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="H110" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G111" s="0" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H111" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G112" s="0" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H112" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G113" s="0" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H113" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G114" s="0" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H114" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G115" s="0" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H115" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G116" s="0" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H116" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G117" s="0" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H117" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G118" s="0" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H118" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G119" s="0" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H119" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G120" s="0" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H120" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G121" s="0" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H121" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G122" s="0" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H122" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G123" s="0" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H123" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G124" s="0" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="H124" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G125" s="0" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="H125" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G126" s="0" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H126" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G127" s="0" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H127" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G128" s="0" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H128" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G129" s="0" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H129" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G130" s="0" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H130" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G131" s="0" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H131" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G132" s="0" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H132" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G133" s="0" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H133" s="0" t="s">
         <v>494</v>
@@ -12074,95 +12052,95 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G134" s="0" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H134" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G135" s="0" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="H135" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G136" s="0" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="H136" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G137" s="0" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="H137" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G138" s="0" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H138" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G139" s="0" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H139" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G140" s="0" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H140" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G141" s="0" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H141" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G142" s="0" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H142" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G143" s="0" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="H143" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G144" s="0" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H144" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G145" s="0" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H145" s="0" t="s">
         <v>492</v>
@@ -12170,7 +12148,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G146" s="0" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H146" s="0" t="s">
         <v>492</v>
@@ -12178,7 +12156,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G147" s="0" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H147" s="0" t="s">
         <v>492</v>
@@ -12186,7 +12164,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G148" s="0" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H148" s="0" t="s">
         <v>492</v>
@@ -12194,7 +12172,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G149" s="0" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H149" s="0" t="s">
         <v>492</v>
@@ -12202,7 +12180,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G150" s="0" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H150" s="0" t="s">
         <v>492</v>
@@ -12210,7 +12188,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G151" s="0" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H151" s="0" t="s">
         <v>494</v>
@@ -12218,7 +12196,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G152" s="0" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H152" s="0" t="s">
         <v>492</v>
@@ -12226,7 +12204,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G153" s="0" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="H153" s="0" t="s">
         <v>492</v>
@@ -12234,7 +12212,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G154" s="0" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="H154" s="0" t="s">
         <v>494</v>
@@ -12242,7 +12220,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G155" s="0" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H155" s="0" t="s">
         <v>494</v>
@@ -12250,7 +12228,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G156" s="0" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H156" s="0" t="s">
         <v>494</v>
@@ -12258,7 +12236,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G157" s="0" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H157" s="0" t="s">
         <v>494</v>
@@ -12266,7 +12244,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G158" s="0" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H158" s="0" t="s">
         <v>494</v>
@@ -12274,7 +12252,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G159" s="0" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="H159" s="0" t="s">
         <v>494</v>
@@ -12389,7 +12367,7 @@
         <v>2302070010</v>
       </c>
       <c r="H173" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12397,7 +12375,7 @@
         <v>2304050000</v>
       </c>
       <c r="H174" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12405,7 +12383,7 @@
         <v>2310022505</v>
       </c>
       <c r="H175" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12413,7 +12391,7 @@
         <v>2311040000</v>
       </c>
       <c r="H176" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12421,7 +12399,7 @@
         <v>2325020000</v>
       </c>
       <c r="H177" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12429,7 +12407,7 @@
         <v>2415005000</v>
       </c>
       <c r="H178" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12437,7 +12415,7 @@
         <v>2415060000</v>
       </c>
       <c r="H179" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>